<commit_message>
Adds changes for cooper's trophy center piece holder.
</commit_message>
<xml_diff>
--- a/2025/Cooper Lorsung/BOM.xlsx
+++ b/2025/Cooper Lorsung/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ppak1\GitHub\Trophy\2025\Cooper Lorsung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A64493C2-845B-47E0-9F39-F903D91E4AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D165C6-A64B-4679-96B3-338055376437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B93C123-BF15-4375-A9C7-2F1595EE499E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Item</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Heat Inserts (Pack of 50)</t>
+  </si>
+  <si>
+    <t>3" Standoff</t>
+  </si>
+  <si>
+    <t>1/2" Ballnose Endmill</t>
   </si>
 </sst>
 </file>
@@ -461,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA25965B-C0B9-4E2E-B0F3-D3F2C80F30B2}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +518,7 @@
       </c>
       <c r="E2">
         <f>SUM(D2:D20)</f>
-        <v>162.29000000000002</v>
+        <v>204.83</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -523,7 +532,7 @@
         <v>11.95</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D9" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D12" si="0">B3*C3</f>
         <v>11.95</v>
       </c>
     </row>
@@ -544,77 +553,122 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" s="2">
-        <v>8.75</v>
+        <v>46.97</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>8.75</v>
+        <v>46.97</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>6.78</v>
+        <v>8.75</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>6.78</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="2">
-        <v>0.81</v>
+        <v>6.78</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.81</v>
+        <v>13.56</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" s="2">
-        <v>15.18</v>
+        <v>0.81</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>15.18</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>15.18</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>15.18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2">
         <v>25.64</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>76.92</v>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>51.28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>9.2100000000000009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2.61</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>5.22</v>
       </c>
     </row>
   </sheetData>
@@ -622,11 +676,14 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{88F92EDB-DFEB-4681-A345-813850B320F3}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{9807EA85-39D1-4BE5-9922-E0F987F13C77}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{E3EDC3CE-9D22-40C5-BF7F-492249A9C2EB}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{E4C61B27-0144-4F6D-A565-B94906884774}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{A97C4495-1401-41B4-9C40-AD26ED4BFF6D}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{9E3AD5E6-49F4-4325-A515-A352801ABF7D}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{FEACE065-C6B2-4149-A022-03083E1EDBF3}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{553564C3-6BC8-4E61-AF06-DD465B281AFF}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{E4C61B27-0144-4F6D-A565-B94906884774}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{A97C4495-1401-41B4-9C40-AD26ED4BFF6D}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{9E3AD5E6-49F4-4325-A515-A352801ABF7D}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{FEACE065-C6B2-4149-A022-03083E1EDBF3}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{553564C3-6BC8-4E61-AF06-DD465B281AFF}"/>
+    <hyperlink ref="A11" r:id="rId9" xr:uid="{8BECD35E-893D-4D8B-A3BE-01AF7BFE3458}"/>
+    <hyperlink ref="A12" r:id="rId10" xr:uid="{022409E4-8FC4-436E-A91E-B57E91CD3CF3}"/>
+    <hyperlink ref="A5" r:id="rId11" xr:uid="{0136E4BC-1DA9-4EDA-899A-43678DD29DC2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>